<commit_message>
Added buffer explosion study and 2kr of throughput in case in case of low interarrival time
</commit_message>
<xml_diff>
--- a/excel/insights/responseTimeInsights.xlsx
+++ b/excel/insights/responseTimeInsights.xlsx
@@ -489,7 +489,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart152.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart160.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -919,11 +919,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="23509631"/>
-        <c:axId val="40332176"/>
+        <c:axId val="71116217"/>
+        <c:axId val="44530271"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23509631"/>
+        <c:axId val="71116217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,12 +979,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40332176"/>
+        <c:crossAx val="44530271"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40332176"/>
+        <c:axId val="44530271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1049,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23509631"/>
+        <c:crossAx val="71116217"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1107,7 +1107,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart153.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart161.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4275,11 +4275,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86317228"/>
-        <c:axId val="64672346"/>
+        <c:axId val="35917865"/>
+        <c:axId val="54797060"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86317228"/>
+        <c:axId val="35917865"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4307,12 +4307,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64672346"/>
+        <c:crossAx val="54797060"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64672346"/>
+        <c:axId val="54797060"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4349,7 +4349,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86317228"/>
+        <c:crossAx val="35917865"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4407,7 +4407,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart154.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart162.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6072,11 +6072,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="95182578"/>
-        <c:axId val="25721729"/>
+        <c:axId val="68353687"/>
+        <c:axId val="87380488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95182578"/>
+        <c:axId val="68353687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6104,12 +6104,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25721729"/>
+        <c:crossAx val="87380488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25721729"/>
+        <c:axId val="87380488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6146,7 +6146,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95182578"/>
+        <c:crossAx val="68353687"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6194,7 +6194,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart155.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart163.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9373,11 +9373,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37827151"/>
-        <c:axId val="10647171"/>
+        <c:axId val="77702419"/>
+        <c:axId val="44792562"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37827151"/>
+        <c:axId val="77702419"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9405,12 +9405,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10647171"/>
+        <c:crossAx val="44792562"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10647171"/>
+        <c:axId val="44792562"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9447,7 +9447,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37827151"/>
+        <c:crossAx val="77702419"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9627,8 +9627,8 @@
   </sheetPr>
   <dimension ref="B1:DN159"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DN82" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DT74" activeCellId="0" sqref="DT74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DN31" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="DR51" activeCellId="0" sqref="DR51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>